<commit_message>
Updated worksheets for alignment to presentation
</commit_message>
<xml_diff>
--- a/data/SG GDP Total and by Industry ANNUAL.xlsx
+++ b/data/SG GDP Total and by Industry ANNUAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8123C131-48F2-459E-B042-F8AE22604839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3725D1D5-D90F-4AED-BAF6-23DBDBB8FF77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2366">
+  <cellXfs count="2367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7583,6 +7583,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7899,7 +7902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BJ82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="BM28" sqref="BM28"/>
     </sheetView>
   </sheetViews>
@@ -17595,7 +17598,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -17609,10 +17612,10 @@
       <c r="A1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2366" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2366" t="s">
         <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -18198,7 +18201,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Updated files according to presentation version
</commit_message>
<xml_diff>
--- a/data/SG GDP Total and by Industry ANNUAL.xlsx
+++ b/data/SG GDP Total and by Industry ANNUAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3725D1D5-D90F-4AED-BAF6-23DBDBB8FF77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB83A13-1741-48ED-B38F-73E22A189B13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17598,7 +17598,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C1" sqref="C1:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -18201,7 +18201,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Updated visualizations into exploratory-analysis.xlsx
</commit_message>
<xml_diff>
--- a/data/SG GDP Total and by Industry ANNUAL.xlsx
+++ b/data/SG GDP Total and by Industry ANNUAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB83A13-1741-48ED-B38F-73E22A189B13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C76CE41-2D52-4D4B-BBF1-10901851167C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -17597,8 +17597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14271DA-2734-4490-A4D3-8CEEE5275FB0}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -18200,8 +18200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAEE12E-E6B0-47B3-8C52-1993CC176FC3}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -18223,6 +18223,7 @@
         <v>2013</v>
       </c>
       <c r="B2" s="2355">
+        <f>SUM('GDP per sector'!D$2:D$18)</f>
         <v>384870.3</v>
       </c>
     </row>
@@ -18231,7 +18232,8 @@
         <v>2014</v>
       </c>
       <c r="B3" s="2355">
-        <v>398947.9</v>
+        <f>SUM('GDP per sector'!E$2:E$18)</f>
+        <v>398947.90000000008</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -18239,6 +18241,7 @@
         <v>2015</v>
       </c>
       <c r="B4" s="2355">
+        <f>SUM('GDP per sector'!F$2:F$18)</f>
         <v>423444.1</v>
       </c>
     </row>
@@ -18247,6 +18250,7 @@
         <v>2016</v>
       </c>
       <c r="B5" s="2355">
+        <f>SUM('GDP per sector'!G$2:G$18)</f>
         <v>440372.2</v>
       </c>
     </row>
@@ -18255,6 +18259,7 @@
         <v>2017</v>
       </c>
       <c r="B6" s="2355">
+        <f>SUM('GDP per sector'!H$2:H$18)</f>
         <v>474115.1</v>
       </c>
     </row>
@@ -18263,7 +18268,8 @@
         <v>2018</v>
       </c>
       <c r="B7" s="2355">
-        <v>507123.9</v>
+        <f>SUM('GDP per sector'!I$2:I$18)</f>
+        <v>507123.89999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -18271,7 +18277,8 @@
         <v>2019</v>
       </c>
       <c r="B8" s="2365">
-        <v>510737.8</v>
+        <f>SUM('GDP per sector'!J$2:J$18)</f>
+        <v>510737.79999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>